<commit_message>
Generate two graphs for the website feature question type
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CAF384-9475-4AF1-B0AC-7A28189C28E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AA29B0-D259-4451-95A6-718D6A28A263}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,12 +222,6 @@
     <t>1,3,5;OO;1</t>
   </si>
   <si>
-    <t>1,2,4;OO;2</t>
-  </si>
-  <si>
-    <t>1,4;OO;3</t>
-  </si>
-  <si>
     <t>1,2,3;OO;2</t>
   </si>
   <si>
@@ -235,6 +229,12 @@
   </si>
   <si>
     <t>1,2;OO;4</t>
+  </si>
+  <si>
+    <t>1,2,4;OC;2</t>
+  </si>
+  <si>
+    <t>1,4;R;3</t>
   </si>
 </sst>
 </file>
@@ -634,13 +634,13 @@
         <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
         <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
         <v>64</v>
@@ -672,19 +672,19 @@
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" t="s">
         <v>68</v>
       </c>
-      <c r="K3" t="s">
-        <v>65</v>
-      </c>
       <c r="L3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" t="s">
         <v>68</v>
-      </c>
-      <c r="M3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
@@ -713,19 +713,19 @@
         <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
         <v>69</v>
       </c>
-      <c r="K4" t="s">
-        <v>66</v>
-      </c>
       <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
         <v>69</v>
-      </c>
-      <c r="M4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
@@ -757,13 +757,13 @@
         <v>64</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
         <v>64</v>
       </c>
       <c r="L5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M5" t="s">
         <v>64</v>
@@ -795,19 +795,19 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" t="s">
         <v>68</v>
       </c>
-      <c r="K6" t="s">
-        <v>65</v>
-      </c>
       <c r="L6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" t="s">
         <v>68</v>
-      </c>
-      <c r="M6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -836,19 +836,19 @@
         <v>45</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" t="s">
         <v>69</v>
       </c>
-      <c r="K7" t="s">
-        <v>66</v>
-      </c>
       <c r="L7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" t="s">
         <v>69</v>
-      </c>
-      <c r="M7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
@@ -880,13 +880,13 @@
         <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s">
         <v>64</v>
       </c>
       <c r="L8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M8" t="s">
         <v>64</v>
@@ -918,19 +918,19 @@
         <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J9" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" t="s">
         <v>68</v>
       </c>
-      <c r="K9" t="s">
-        <v>65</v>
-      </c>
       <c r="L9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" t="s">
         <v>68</v>
-      </c>
-      <c r="M9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -959,19 +959,19 @@
         <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" t="s">
         <v>69</v>
       </c>
-      <c r="K10" t="s">
-        <v>66</v>
-      </c>
       <c r="L10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" t="s">
         <v>69</v>
-      </c>
-      <c r="M10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -1003,13 +1003,13 @@
         <v>64</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
         <v>64</v>
       </c>
       <c r="L11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M11" t="s">
         <v>64</v>
@@ -1041,19 +1041,19 @@
         <v>45</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" t="s">
         <v>68</v>
       </c>
-      <c r="K12" t="s">
-        <v>65</v>
-      </c>
       <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
         <v>68</v>
-      </c>
-      <c r="M12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -1082,19 +1082,19 @@
         <v>45</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" t="s">
         <v>69</v>
       </c>
-      <c r="K13" t="s">
-        <v>66</v>
-      </c>
       <c r="L13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" t="s">
         <v>69</v>
-      </c>
-      <c r="M13" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -1126,13 +1126,13 @@
         <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
         <v>64</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M14" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Fix issues caused by empty text
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AA29B0-D259-4451-95A6-718D6A28A263}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23B5961-8C39-4765-8793-B993A0CA256D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
   <si>
     <t>1;2;3;4</t>
   </si>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>Product should be improved</t>
-  </si>
-  <si>
-    <t>Nil</t>
   </si>
   <si>
     <t>Utilisation Portal needs improvements</t>
@@ -560,7 +557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -590,19 +589,19 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
@@ -631,19 +630,19 @@
         <v>45</v>
       </c>
       <c r="I2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" t="s">
         <v>64</v>
       </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
       <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
         <v>64</v>
       </c>
-      <c r="L2" t="s">
-        <v>65</v>
-      </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -672,19 +671,19 @@
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
@@ -713,19 +712,19 @@
         <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
@@ -754,19 +753,19 @@
         <v>45</v>
       </c>
       <c r="I5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" t="s">
         <v>64</v>
       </c>
-      <c r="J5" t="s">
-        <v>65</v>
-      </c>
       <c r="K5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" t="s">
         <v>64</v>
       </c>
-      <c r="L5" t="s">
-        <v>65</v>
-      </c>
       <c r="M5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
@@ -779,9 +778,6 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
       <c r="E6">
         <v>5</v>
       </c>
@@ -795,19 +791,19 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -821,7 +817,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -836,19 +832,19 @@
         <v>45</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
@@ -877,19 +873,19 @@
         <v>46</v>
       </c>
       <c r="I8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" t="s">
         <v>64</v>
       </c>
-      <c r="J8" t="s">
-        <v>65</v>
-      </c>
       <c r="K8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" t="s">
         <v>64</v>
       </c>
-      <c r="L8" t="s">
-        <v>65</v>
-      </c>
       <c r="M8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
@@ -918,19 +914,19 @@
         <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -944,7 +940,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -959,19 +955,19 @@
         <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -985,7 +981,7 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -1000,19 +996,19 @@
         <v>45</v>
       </c>
       <c r="I11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" t="s">
         <v>64</v>
       </c>
-      <c r="J11" t="s">
-        <v>65</v>
-      </c>
       <c r="K11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" t="s">
         <v>64</v>
       </c>
-      <c r="L11" t="s">
-        <v>65</v>
-      </c>
       <c r="M11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
@@ -1026,7 +1022,7 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1041,19 +1037,19 @@
         <v>45</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -1082,19 +1078,19 @@
         <v>45</v>
       </c>
       <c r="I13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -1123,19 +1119,19 @@
         <v>47</v>
       </c>
       <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" t="s">
         <v>64</v>
       </c>
-      <c r="J14" t="s">
-        <v>65</v>
-      </c>
       <c r="K14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" t="s">
         <v>64</v>
       </c>
-      <c r="L14" t="s">
-        <v>65</v>
-      </c>
       <c r="M14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>